<commit_message>
Updated the area vise equipments
</commit_message>
<xml_diff>
--- a/bina_refinery_log.xlsx
+++ b/bina_refinery_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>Timestamp</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +494,8 @@
           <t>2025-05-26 20:23:40</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -509,6 +521,35 @@
           <t>2025-05-26 20:24:00</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Crude Distillation Unit (CDU)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Top Temperature</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-05-27 10:22:43</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>